<commit_message>
Inventory:Feat: Excel con sender _id y relación movementPending
</commit_message>
<xml_diff>
--- a/public/upload-template/carga_inventario.xlsx
+++ b/public/upload-template/carga_inventario.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Alpine16\home\atorres\ionline\public\upload-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBC9E56-B474-440D-B09D-0BEC1B80216E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C211D-2ED7-41B9-96FF-301E9B9896F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="base note book inicial" sheetId="1" r:id="rId1"/>
+    <sheet name="carga_masiva_inventario" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'base note book inicial'!$A$1:$P$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">carga_masiva_inventario!$A$1:$Q$70</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>marca</t>
   </si>
@@ -108,15 +108,6 @@
     <t>BUENO</t>
   </si>
   <si>
-    <t>20505776</t>
-  </si>
-  <si>
-    <t>13866449</t>
-  </si>
-  <si>
-    <t>16592972</t>
-  </si>
-  <si>
     <t>valor</t>
   </si>
   <si>
@@ -144,9 +135,6 @@
     <t>obligatorio (unspsc_product_id)</t>
   </si>
   <si>
-    <t>obligatorio (-1, 0, 1) Malo, Regular, Bueno</t>
-  </si>
-  <si>
     <t>vida_util</t>
   </si>
   <si>
@@ -160,13 +148,23 @@
   </si>
   <si>
     <t>Tiene el vidrio roto</t>
+  </si>
+  <si>
+    <t>quien entrega</t>
+  </si>
+  <si>
+    <t>opcional - el usuario que está entregando el bien a el responsable</t>
+  </si>
+  <si>
+    <t>obligatorio 
+Malo, Regular, Bueno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,14 +185,6 @@
       <color rgb="FF212529"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -272,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -282,26 +272,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,11 +604,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -635,16 +620,17 @@
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -664,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>7</v>
@@ -676,28 +662,31 @@
         <v>6</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="O1" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -705,7 +694,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>4</v>
@@ -718,37 +707,40 @@
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="M2" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="O2" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -776,27 +768,27 @@
       <c r="J3">
         <v>1132</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" t="s">
-        <v>43</v>
-      </c>
-      <c r="N3">
+      <c r="L3" s="2">
+        <v>15287582</v>
+      </c>
+      <c r="M3" s="2">
+        <v>20505776</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3">
         <v>180880</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>5320413</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>8555</v>
       </c>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -824,26 +816,29 @@
       <c r="J4">
         <v>1132</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4">
+      <c r="K4" s="2">
+        <v>16592972</v>
+      </c>
+      <c r="L4" s="2">
+        <v>15287582</v>
+      </c>
+      <c r="M4" s="2">
+        <v>13866449</v>
+      </c>
+      <c r="O4">
         <v>180880</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>5320413</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>8555</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="3">
         <v>45006</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -871,543 +866,543 @@
       <c r="J5">
         <v>1132</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5">
+      <c r="L5" s="2">
+        <v>16592972</v>
+      </c>
+      <c r="M5" s="2">
+        <v>16592972</v>
+      </c>
+      <c r="O5">
         <v>180880</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>5320413</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>8555</v>
       </c>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="I11" s="2"/>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="I13" s="2"/>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="I16" s="2"/>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="I17" s="2"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="I18" s="2"/>
-      <c r="Q18" s="3"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="Q19" s="3"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="Q20" s="3"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="I21" s="2"/>
-      <c r="Q21" s="3"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="I22" s="2"/>
-      <c r="Q22" s="3"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="Q23" s="3"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="I24" s="2"/>
-      <c r="Q24" s="3"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24" s="3"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="I25" s="2"/>
-      <c r="Q25" s="3"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="I26" s="2"/>
-      <c r="Q26" s="3"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="I27" s="2"/>
-      <c r="Q27" s="3"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27" s="3"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="I28" s="2"/>
-      <c r="Q28" s="3"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28" s="3"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="I29" s="2"/>
-      <c r="Q29" s="3"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="I30" s="2"/>
-      <c r="Q30" s="3"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30" s="3"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="I31" s="2"/>
-      <c r="Q31" s="3"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31" s="3"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="Q32" s="3"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32" s="3"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="Q33" s="3"/>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33" s="3"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="Q34" s="3"/>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34" s="3"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="Q35" s="3"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35" s="3"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="I36" s="2"/>
-      <c r="Q36" s="3"/>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36" s="3"/>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="I37" s="2"/>
-      <c r="Q37" s="3"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37" s="3"/>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="I38" s="2"/>
-      <c r="Q38" s="3"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38" s="3"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="I39" s="2"/>
-      <c r="Q39" s="3"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39" s="3"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="I40" s="2"/>
-      <c r="Q40" s="3"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40" s="3"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="I41" s="2"/>
-      <c r="Q41" s="3"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41" s="3"/>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="Q42" s="3"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42" s="3"/>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="I43" s="2"/>
-      <c r="Q43" s="3"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43" s="3"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="I44" s="2"/>
-      <c r="Q44" s="3"/>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44" s="3"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="I45" s="2"/>
-      <c r="Q45" s="3"/>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45" s="3"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="Q46" s="3"/>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46" s="3"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
       <c r="I47" s="2"/>
-      <c r="Q47" s="3"/>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47" s="3"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
       <c r="I48" s="2"/>
-      <c r="Q48" s="3"/>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48" s="3"/>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="I49" s="2"/>
-      <c r="Q49" s="3"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49" s="3"/>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="I50" s="2"/>
-      <c r="Q50" s="3"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50" s="3"/>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
       <c r="I51" s="2"/>
-      <c r="Q51" s="3"/>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R51" s="3"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
       <c r="I52" s="2"/>
-      <c r="Q52" s="3"/>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R52" s="3"/>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="Q53" s="3"/>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53" s="3"/>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="Q54" s="3"/>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R54" s="3"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
       <c r="I55" s="2"/>
-      <c r="Q55" s="3"/>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R55" s="3"/>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
       <c r="I56" s="2"/>
-      <c r="Q56" s="3"/>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56" s="3"/>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="Q57" s="3"/>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R57" s="3"/>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="Q58" s="3"/>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R58" s="3"/>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
       <c r="I59" s="2"/>
-      <c r="Q59" s="3"/>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R59" s="3"/>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
       <c r="I60" s="2"/>
-      <c r="Q60" s="3"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R60" s="3"/>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
       <c r="I61" s="2"/>
-      <c r="Q61" s="3"/>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R61" s="3"/>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="I62" s="2"/>
-      <c r="Q62" s="3"/>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R62" s="3"/>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="I63" s="2"/>
-      <c r="Q63" s="3"/>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R63" s="3"/>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="I64" s="2"/>
-      <c r="Q64" s="3"/>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R64" s="3"/>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="I65" s="2"/>
-      <c r="Q65" s="3"/>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R65" s="3"/>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="I66" s="2"/>
-      <c r="Q66" s="3"/>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R66" s="3"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="I67" s="2"/>
-      <c r="Q67" s="3"/>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R67" s="3"/>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="I68" s="2"/>
-      <c r="Q68" s="3"/>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R68" s="3"/>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="I69" s="2"/>
-      <c r="Q69" s="3"/>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R69" s="3"/>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="I70" s="2"/>
-      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
con excel old_value y carga de este, fix ident
</commit_message>
<xml_diff>
--- a/public/upload-template/carga_inventario.xlsx
+++ b/public/upload-template/carga_inventario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Alpine16\home\atorres\ionline\public\upload-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tebi\Desarrollo\ionline\public\upload-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220C211D-2ED7-41B9-96FF-301E9B9896F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FE1A7E-53EA-43B5-B1BE-E82E52D28858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="carga_masiva_inventario" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>marca</t>
   </si>
@@ -158,6 +158,12 @@
   <si>
     <t>obligatorio 
 Malo, Regular, Bueno</t>
+  </si>
+  <si>
+    <t>opcional, ya no se ocupa, Numero de inventario antiguo</t>
+  </si>
+  <si>
+    <t>old number</t>
   </si>
 </sst>
 </file>
@@ -604,9 +610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R70"/>
+  <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -627,10 +635,11 @@
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" customWidth="1"/>
+    <col min="18" max="18" width="21" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
@@ -685,8 +694,11 @@
       <c r="R1" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.25">
+      <c r="S1" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -739,8 +751,11 @@
       <c r="R2" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -787,8 +802,9 @@
         <v>8555</v>
       </c>
       <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="3"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -837,8 +853,9 @@
       <c r="R4" s="3">
         <v>45006</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="3"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -882,8 +899,9 @@
         <v>8555</v>
       </c>
       <c r="R5" s="3"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="3"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
@@ -891,7 +909,7 @@
       <c r="I6" s="2"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
@@ -900,7 +918,7 @@
       <c r="I7" s="2"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="D8" s="2"/>
@@ -908,7 +926,7 @@
       <c r="I8" s="2"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>
@@ -916,7 +934,7 @@
       <c r="I9" s="2"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
@@ -924,7 +942,7 @@
       <c r="I10" s="2"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
@@ -932,7 +950,7 @@
       <c r="I11" s="2"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
@@ -940,7 +958,7 @@
       <c r="I12" s="2"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
@@ -948,7 +966,7 @@
       <c r="I13" s="2"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
@@ -956,7 +974,7 @@
       <c r="I14" s="2"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
@@ -964,7 +982,7 @@
       <c r="I15" s="2"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
con el campo clasificacion
</commit_message>
<xml_diff>
--- a/public/upload-template/carga_inventario.xlsx
+++ b/public/upload-template/carga_inventario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tebi\Desarrollo\ionline\public\upload-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E25BC8C-0740-4ABF-A9D4-1374B76F759B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B759D998-9A1E-49C5-9868-0252078D50C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>marca</t>
   </si>
@@ -164,6 +164,16 @@
   </si>
   <si>
     <t>opcional, en caso que no se digite se creara un numero de inventario nuevo. En caso de actualizar caracteristicas de un inventario se debe digitar</t>
+  </si>
+  <si>
+    <t>clasificacion</t>
+  </si>
+  <si>
+    <t>opcional
+1= HAH
+2 = ADM
+3 = SAS
+4 = COM</t>
   </si>
 </sst>
 </file>
@@ -610,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S70"/>
+  <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +649,7 @@
     <col min="19" max="19" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
@@ -697,8 +707,11 @@
       <c r="S1" s="10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="5" customFormat="1" ht="96" x14ac:dyDescent="0.25">
+      <c r="T1" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="5" customFormat="1" ht="96" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>44</v>
       </c>
@@ -754,8 +767,11 @@
       <c r="S2" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T2" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -803,8 +819,11 @@
       </c>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -855,7 +874,7 @@
       </c>
       <c r="S4" s="3"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
@@ -901,7 +920,7 @@
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="D6" s="2"/>
@@ -909,7 +928,7 @@
       <c r="I6" s="2"/>
       <c r="R6" s="3"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
@@ -918,7 +937,7 @@
       <c r="I7" s="2"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="D8" s="2"/>
@@ -926,7 +945,7 @@
       <c r="I8" s="2"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="D9" s="2"/>
@@ -934,7 +953,7 @@
       <c r="I9" s="2"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="D10" s="2"/>
@@ -942,7 +961,7 @@
       <c r="I10" s="2"/>
       <c r="R10" s="3"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="D11" s="2"/>
@@ -950,7 +969,7 @@
       <c r="I11" s="2"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="D12" s="2"/>
@@ -958,7 +977,7 @@
       <c r="I12" s="2"/>
       <c r="R12" s="3"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="D13" s="2"/>
@@ -966,7 +985,7 @@
       <c r="I13" s="2"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="D14" s="2"/>
@@ -974,7 +993,7 @@
       <c r="I14" s="2"/>
       <c r="R14" s="3"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="D15" s="2"/>
@@ -982,7 +1001,7 @@
       <c r="I15" s="2"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
mejor texto excel y validaciones individuales
</commit_message>
<xml_diff>
--- a/public/upload-template/carga_inventario.xlsx
+++ b/public/upload-template/carga_inventario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tebi\Desarrollo\ionline\public\upload-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B759D998-9A1E-49C5-9868-0252078D50C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2CB340-3605-4985-B4E1-2EED4B9D63C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>marca</t>
   </si>
@@ -141,16 +141,10 @@
     <t>opcional, si se ingresa, aparecerá confirmado por el responsable (reception_date)</t>
   </si>
   <si>
-    <t>opcional (si no existe el usuario no se creará el registro)</t>
-  </si>
-  <si>
     <t>Tiene el vidrio roto</t>
   </si>
   <si>
     <t>quien entrega</t>
-  </si>
-  <si>
-    <t>opcional - el usuario que está entregando el bien a el responsable</t>
   </si>
   <si>
     <t>obligatorio 
@@ -174,6 +168,18 @@
 2 = ADM
 3 = SAS
 4 = COM</t>
+  </si>
+  <si>
+    <t>obligatorio para generar movimiento
+(el usuario que está entregando el bien)</t>
+  </si>
+  <si>
+    <t>obligatorio para generar movimiento
+si no existe el usuario responsable no se creará el registro</t>
+  </si>
+  <si>
+    <t>obligatorio para generar movimiento
+Usuario que utilizará el bien</t>
   </si>
 </sst>
 </file>
@@ -225,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +253,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -304,6 +316,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -623,7 +641,7 @@
   <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +699,7 @@
         <v>5</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>13</v>
@@ -705,15 +723,15 @@
         <v>35</v>
       </c>
       <c r="S1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:20" s="5" customFormat="1" ht="96" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>3</v>
@@ -735,19 +753,19 @@
         <v>32</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>37</v>
+      <c r="K2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>47</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>4</v>
@@ -765,10 +783,10 @@
         <v>36</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -799,6 +817,9 @@
       <c r="J3">
         <v>1132</v>
       </c>
+      <c r="K3" s="2">
+        <v>15287582</v>
+      </c>
       <c r="L3" s="2">
         <v>15287582</v>
       </c>
@@ -806,7 +827,7 @@
         <v>20505776</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O3">
         <v>180880</v>
@@ -901,6 +922,9 @@
       </c>
       <c r="J5">
         <v>1132</v>
+      </c>
+      <c r="K5" s="2">
+        <v>16592972</v>
       </c>
       <c r="L5" s="2">
         <v>16592972</v>

</xml_diff>

<commit_message>
inventory: se modifican modulos que dependen de usuario para activar multiusuario
</commit_message>
<xml_diff>
--- a/public/upload-template/carga_inventario.xlsx
+++ b/public/upload-template/carga_inventario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tebi\Desarrollo\ionline\public\upload-template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2CB340-3605-4985-B4E1-2EED4B9D63C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87568BBC-A70D-4552-A4DD-2D8908E153D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,8 +178,7 @@
 si no existe el usuario responsable no se creará el registro</t>
   </si>
   <si>
-    <t>obligatorio para generar movimiento
-Usuario que utilizará el bien</t>
+    <t>Ya no se utiliza debido a que ahora es multuusuario</t>
   </si>
 </sst>
 </file>
@@ -342,9 +341,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -382,7 +381,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -488,7 +487,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -630,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -641,7 +640,7 @@
   <dimension ref="A1:T70"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>